<commit_message>
Testovi edit name of account
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="4356"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>username</t>
   </si>
@@ -38,10 +38,16 @@
     <t>isMock</t>
   </si>
   <si>
+    <t>personal_account_iban</t>
+  </si>
+  <si>
     <t>Osir ANOEV</t>
   </si>
   <si>
     <t>ART02</t>
+  </si>
+  <si>
+    <t>205-9031004417882-84</t>
   </si>
 </sst>
 </file>
@@ -983,20 +989,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="17.712962962963" style="1" customWidth="1"/>
     <col min="2" max="2" width="33.5740740740741" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88888888888889" style="1"/>
+    <col min="3" max="3" width="8.88888888888889" style="1"/>
+    <col min="4" max="4" width="28.5555555555556" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:3">
+    <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1006,16 +1014,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Product Summary testovi da promenu imena producta, dodat Aleksin da se menja za vise razlicitih prodatka
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10187"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>username</t>
   </si>
@@ -53,6 +53,12 @@
     <t>personal_name</t>
   </si>
   <si>
+    <t>personal_account_iban1</t>
+  </si>
+  <si>
+    <t>personal_account_name1</t>
+  </si>
+  <si>
     <t>personal_account_iban2</t>
   </si>
   <si>
@@ -65,6 +71,36 @@
     <t>personal_account_name3</t>
   </si>
   <si>
+    <t>credit_card_1_name</t>
+  </si>
+  <si>
+    <t>credit_card_1_bban</t>
+  </si>
+  <si>
+    <t>credit_card_2_name</t>
+  </si>
+  <si>
+    <t>credit_card_2_bban</t>
+  </si>
+  <si>
+    <t>savings_account_1_name</t>
+  </si>
+  <si>
+    <t>savings_account_1_bban</t>
+  </si>
+  <si>
+    <t>savings_account_2_name</t>
+  </si>
+  <si>
+    <t>savings_account_2_bban</t>
+  </si>
+  <si>
+    <t>term_deposit_1_name</t>
+  </si>
+  <si>
+    <t>term_deposits_1_bban</t>
+  </si>
+  <si>
     <t>Osir ANOEV</t>
   </si>
   <si>
@@ -93,6 +129,33 @@
   </si>
   <si>
     <t>Payment account with basic services</t>
+  </si>
+  <si>
+    <t>Visa prepaid</t>
+  </si>
+  <si>
+    <t>4431 3*** **** *011 8</t>
+  </si>
+  <si>
+    <t>Visa revolving card</t>
+  </si>
+  <si>
+    <t>4176 **** **** 8476</t>
+  </si>
+  <si>
+    <t>A vista deposit account</t>
+  </si>
+  <si>
+    <t>205-9011008384007-23</t>
+  </si>
+  <si>
+    <t>205-9011008395360-11</t>
+  </si>
+  <si>
+    <t>Term deposits</t>
+  </si>
+  <si>
+    <t>205-9032022325800-66</t>
   </si>
   <si>
     <t>Drre ĆEVMI</t>
@@ -1081,10 +1144,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
@@ -1098,13 +1161,25 @@
     <col min="7" max="7" width="36.1111111111111" style="1" customWidth="1"/>
     <col min="8" max="8" width="28.4444444444444" style="1" customWidth="1"/>
     <col min="9" max="9" width="23.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="35.1111111111111" style="1" customWidth="1"/>
-    <col min="11" max="11" width="38.3333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="30.1111111111111" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88888888888889" style="1"/>
+    <col min="10" max="10" width="33" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.3333333333333" style="1" customWidth="1"/>
+    <col min="12" max="12" width="35.1111111111111" style="1" customWidth="1"/>
+    <col min="13" max="13" width="38.3333333333333" style="1" customWidth="1"/>
+    <col min="14" max="14" width="30.1111111111111" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5555555555556" style="1" customWidth="1"/>
+    <col min="16" max="16" width="21.7777777777778" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5555555555556" style="1" customWidth="1"/>
+    <col min="18" max="18" width="18.8888888888889" style="1" customWidth="1"/>
+    <col min="19" max="19" width="24.1111111111111" style="1" customWidth="1"/>
+    <col min="20" max="20" width="23.5555555555556" style="1" customWidth="1"/>
+    <col min="21" max="21" width="24.1111111111111" style="1" customWidth="1"/>
+    <col min="22" max="22" width="23.5555555555556" style="1" customWidth="1"/>
+    <col min="23" max="23" width="21.4444444444444" style="1" customWidth="1"/>
+    <col min="24" max="24" width="21.6666666666667" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:12">
+    <row r="1" s="1" customFormat="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1141,68 +1216,140 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="39.6" spans="1:12">
+    <row r="2" s="1" customFormat="1" ht="39.6" spans="1:24">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="3" ht="28.8" spans="1:11">
+    <row r="3" ht="28.8" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="M3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Foreign Current AccountProduct Details Account Details
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>username</t>
   </si>
@@ -50,6 +50,9 @@
     <t>personal_account_number</t>
   </si>
   <si>
+    <t>personal_account_number2</t>
+  </si>
+  <si>
     <t>personal_name</t>
   </si>
   <si>
@@ -117,6 +120,9 @@
   </si>
   <si>
     <t>RS35 2059 0310 0441 9532 81</t>
+  </si>
+  <si>
+    <t>RS35 2059 0310 0441 7882 84</t>
   </si>
   <si>
     <t>OSIR ANOEV</t>
@@ -1144,10 +1150,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
@@ -1159,27 +1165,27 @@
     <col min="5" max="5" width="71.2222222222222" style="1" customWidth="1"/>
     <col min="6" max="6" width="125.222222222222" style="1" customWidth="1"/>
     <col min="7" max="7" width="36.1111111111111" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.4444444444444" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="33" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.3333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="35.1111111111111" style="1" customWidth="1"/>
-    <col min="13" max="13" width="38.3333333333333" style="1" customWidth="1"/>
-    <col min="14" max="14" width="30.1111111111111" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5555555555556" style="1" customWidth="1"/>
-    <col min="16" max="16" width="21.7777777777778" style="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5555555555556" style="1" customWidth="1"/>
-    <col min="18" max="18" width="18.8888888888889" style="1" customWidth="1"/>
-    <col min="19" max="19" width="24.1111111111111" style="1" customWidth="1"/>
-    <col min="20" max="20" width="23.5555555555556" style="1" customWidth="1"/>
-    <col min="21" max="21" width="24.1111111111111" style="1" customWidth="1"/>
-    <col min="22" max="22" width="23.5555555555556" style="1" customWidth="1"/>
-    <col min="23" max="23" width="21.4444444444444" style="1" customWidth="1"/>
-    <col min="24" max="24" width="21.6666666666667" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.88888888888889" style="1"/>
+    <col min="8" max="9" width="28.4444444444444" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.3333333333333" style="1" customWidth="1"/>
+    <col min="11" max="11" width="33" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.3333333333333" style="1" customWidth="1"/>
+    <col min="13" max="13" width="35.1111111111111" style="1" customWidth="1"/>
+    <col min="14" max="14" width="38.3333333333333" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.1111111111111" style="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5555555555556" style="1" customWidth="1"/>
+    <col min="17" max="17" width="21.7777777777778" style="1" customWidth="1"/>
+    <col min="18" max="18" width="19.5555555555556" style="1" customWidth="1"/>
+    <col min="19" max="19" width="18.8888888888889" style="1" customWidth="1"/>
+    <col min="20" max="20" width="24.1111111111111" style="1" customWidth="1"/>
+    <col min="21" max="21" width="23.5555555555556" style="1" customWidth="1"/>
+    <col min="22" max="22" width="24.1111111111111" style="1" customWidth="1"/>
+    <col min="23" max="23" width="23.5555555555556" style="1" customWidth="1"/>
+    <col min="24" max="24" width="21.4444444444444" style="1" customWidth="1"/>
+    <col min="25" max="25" width="21.6666666666667" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:24">
+    <row r="1" s="1" customFormat="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1252,104 +1258,110 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="39.6" spans="1:24">
+    <row r="2" s="1" customFormat="1" ht="39.6" spans="1:25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="3" ht="28.8" spans="1:13">
+    <row r="3" ht="28.8" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="N3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
U testu create conformation dinamicka putanja umesto hardkodovane
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10187"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>username</t>
   </si>
@@ -104,9 +104,6 @@
     <t>term_deposits_1_bban</t>
   </si>
   <si>
-    <t>pdf_download_path</t>
-  </si>
-  <si>
     <t>Osir ANOEV</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
   </si>
   <si>
     <t>205-9032022325800-66</t>
-  </si>
-  <si>
-    <t>C:\Users\Jelena Bulajic\Downloads</t>
   </si>
   <si>
     <t>Drre ĆEVMI</t>
@@ -1167,7 +1161,7 @@
   <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
@@ -1276,111 +1270,106 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="6"/>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="39.6" spans="1:25">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="39.6" spans="1:26">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" ht="28.8" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="N3" s="5"/>
     </row>

</xml_diff>

<commit_message>
Cetrdeset sedam testova konacno
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10187"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="56">
   <si>
     <t>username</t>
   </si>
@@ -38,120 +38,120 @@
     <t>isMock</t>
   </si>
   <si>
+    <t>current_account_1_name</t>
+  </si>
+  <si>
+    <t>current_account_1_number</t>
+  </si>
+  <si>
+    <t>current_account_1_bban</t>
+  </si>
+  <si>
+    <t>current_account_2_name</t>
+  </si>
+  <si>
+    <t>current_account_2_bban</t>
+  </si>
+  <si>
+    <t>current_account_3_name</t>
+  </si>
+  <si>
+    <t>current_account_3_bban</t>
+  </si>
+  <si>
+    <t>credit_card_1_name</t>
+  </si>
+  <si>
+    <t>credit_card_1_bban</t>
+  </si>
+  <si>
+    <t>credit_card_2_name</t>
+  </si>
+  <si>
+    <t>credit_card_2_bban</t>
+  </si>
+  <si>
+    <t>savings_account_1_name</t>
+  </si>
+  <si>
+    <t>savings_account_1_bban</t>
+  </si>
+  <si>
+    <t>savings_account_2_name</t>
+  </si>
+  <si>
+    <t>savings_account_2_bban</t>
+  </si>
+  <si>
+    <t>term_deposit_1_name</t>
+  </si>
+  <si>
+    <t>term_deposits_1_bban</t>
+  </si>
+  <si>
+    <t>cardName</t>
+  </si>
+  <si>
+    <t>default_account_bban</t>
+  </si>
+  <si>
     <t>copied_account_details_for_personal_account</t>
   </si>
   <si>
-    <t>current_account_1_name</t>
-  </si>
-  <si>
-    <t>current_account_1_number</t>
-  </si>
-  <si>
-    <t>current_account_1_bban</t>
-  </si>
-  <si>
-    <t>current_account_2_name</t>
-  </si>
-  <si>
-    <t>current_account_2_bban</t>
-  </si>
-  <si>
-    <t>current_account_3_name</t>
-  </si>
-  <si>
-    <t>current_account_3_bban</t>
-  </si>
-  <si>
-    <t>credit_card_1_name</t>
-  </si>
-  <si>
-    <t>credit_card_1_bban</t>
-  </si>
-  <si>
-    <t>credit_card_2_name</t>
-  </si>
-  <si>
-    <t>credit_card_2_bban</t>
-  </si>
-  <si>
-    <t>savings_account_1_name</t>
-  </si>
-  <si>
-    <t>savings_account_1_bban</t>
-  </si>
-  <si>
-    <t>savings_account_2_name</t>
-  </si>
-  <si>
-    <t>savings_account_2_bban</t>
-  </si>
-  <si>
-    <t>term_deposit_1_name</t>
-  </si>
-  <si>
-    <t>term_deposits_1_bban</t>
-  </si>
-  <si>
-    <t>cardName</t>
-  </si>
-  <si>
-    <t>default_account_bban</t>
-  </si>
-  <si>
     <t>Osir ANOEV</t>
   </si>
   <si>
     <t>ART02</t>
   </si>
   <si>
+    <t>Devizni platni račun</t>
+  </si>
+  <si>
+    <t>RS35 2059 0310 0441 7882 84</t>
+  </si>
+  <si>
+    <t>205-9031004417882-84</t>
+  </si>
+  <si>
+    <t>Tekući račun</t>
+  </si>
+  <si>
+    <t>205-9001007790944-88</t>
+  </si>
+  <si>
+    <t>205-9031004419532-81</t>
+  </si>
+  <si>
+    <t>Visa prepaid</t>
+  </si>
+  <si>
+    <t>4431 3*** **** *011 8</t>
+  </si>
+  <si>
+    <t>Visa revolving card</t>
+  </si>
+  <si>
+    <t>4176 **** **** 8476</t>
+  </si>
+  <si>
+    <t>A vista deposit account</t>
+  </si>
+  <si>
+    <t>205-9011008384007-23</t>
+  </si>
+  <si>
+    <t>205-9011008395360-11</t>
+  </si>
+  <si>
+    <t>Term deposits</t>
+  </si>
+  <si>
+    <t>205-9032022325800-66</t>
+  </si>
+  <si>
     <t xml:space="preserve">Account type: Current account Account owner: OSIR ANOEV Account number: RS35 2059 0310 0441 7882 84 BIC: KOBBRSBG </t>
   </si>
   <si>
-    <t>Devizni platni račun</t>
-  </si>
-  <si>
-    <t>RS35 2059 0310 0441 7882 84</t>
-  </si>
-  <si>
-    <t>205-9031004417882-84</t>
-  </si>
-  <si>
-    <t>Tekući račun</t>
-  </si>
-  <si>
-    <t>205-9001007790944-88</t>
-  </si>
-  <si>
-    <t>205-9031004419532-81</t>
-  </si>
-  <si>
-    <t>Visa prepaid</t>
-  </si>
-  <si>
-    <t>4431 3*** **** *011 8</t>
-  </si>
-  <si>
-    <t>Visa revolving card</t>
-  </si>
-  <si>
-    <t>4176 **** **** 8476</t>
-  </si>
-  <si>
-    <t>A vista deposit account</t>
-  </si>
-  <si>
-    <t>205-9011008384007-23</t>
-  </si>
-  <si>
-    <t>205-9011008395360-11</t>
-  </si>
-  <si>
-    <t>Term deposits</t>
-  </si>
-  <si>
-    <t>205-9032022325800-66</t>
-  </si>
-  <si>
     <t>Enil ČIĆVI</t>
   </si>
   <si>
@@ -179,10 +179,22 @@
     <t>Drre ĆEVMI</t>
   </si>
   <si>
+    <t>205-9031002637397-40</t>
+  </si>
+  <si>
     <t xml:space="preserve">Account type: Current account Account owner: DRRE ĆEVMI Account number: RS35 2059 0310 0263 7397 40 BIC: KOBBRSBG </t>
   </si>
   <si>
-    <t>205-9031002637397-40</t>
+    <t>Jail ĆEVGIMILĆ</t>
+  </si>
+  <si>
+    <t>205-9001007668260-25</t>
+  </si>
+  <si>
+    <t>Veli NACMI</t>
+  </si>
+  <si>
+    <t>205-9001007159209-10</t>
   </si>
 </sst>
 </file>
@@ -822,7 +834,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -843,6 +855,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -1380,34 +1395,35 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="17.712962962963" style="3" customWidth="1"/>
     <col min="2" max="2" width="33.5740740740741" style="3" customWidth="1"/>
     <col min="3" max="3" width="8.88888888888889" style="3"/>
-    <col min="4" max="4" width="114.666666666667" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33" style="3" customWidth="1"/>
-    <col min="6" max="7" width="114.777777777778" style="3" customWidth="1"/>
-    <col min="8" max="8" width="33.8888888888889" style="3" customWidth="1"/>
-    <col min="9" max="9" width="23.6666666666667" style="3" customWidth="1"/>
-    <col min="10" max="12" width="24.2222222222222" style="3" customWidth="1"/>
-    <col min="13" max="13" width="23.6666666666667" style="3" customWidth="1"/>
-    <col min="14" max="14" width="19.5555555555556" style="3" customWidth="1"/>
-    <col min="15" max="15" width="18.8888888888889" style="3" customWidth="1"/>
-    <col min="16" max="16" width="24.1111111111111" style="3" customWidth="1"/>
-    <col min="17" max="17" width="23.5555555555556" style="3" customWidth="1"/>
-    <col min="18" max="18" width="24.1111111111111" style="3" customWidth="1"/>
-    <col min="19" max="19" width="23.5555555555556" style="3" customWidth="1"/>
-    <col min="20" max="20" width="24.1111111111111" style="3" customWidth="1"/>
-    <col min="21" max="21" width="23.5555555555556" style="3" customWidth="1"/>
-    <col min="22" max="22" width="17.6666666666667" style="3" customWidth="1"/>
-    <col min="23" max="23" width="23.8888888888889" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33" style="3" customWidth="1"/>
+    <col min="5" max="5" width="26.1111111111111" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.6666666666667" style="3" customWidth="1"/>
+    <col min="7" max="7" width="33.8888888888889" style="3" customWidth="1"/>
+    <col min="8" max="8" width="23.6666666666667" style="3" customWidth="1"/>
+    <col min="9" max="11" width="24.2222222222222" style="3" customWidth="1"/>
+    <col min="12" max="12" width="23.6666666666667" style="3" customWidth="1"/>
+    <col min="13" max="13" width="19.5555555555556" style="3" customWidth="1"/>
+    <col min="14" max="14" width="18.8888888888889" style="3" customWidth="1"/>
+    <col min="15" max="15" width="24.1111111111111" style="3" customWidth="1"/>
+    <col min="16" max="16" width="23.5555555555556" style="3" customWidth="1"/>
+    <col min="17" max="17" width="24.1111111111111" style="3" customWidth="1"/>
+    <col min="18" max="18" width="23.5555555555556" style="3" customWidth="1"/>
+    <col min="19" max="19" width="24.1111111111111" style="3" customWidth="1"/>
+    <col min="20" max="20" width="23.5555555555556" style="3" customWidth="1"/>
+    <col min="21" max="21" width="17.6666666666667" style="3" customWidth="1"/>
+    <col min="22" max="22" width="23.8888888888889" style="3" customWidth="1"/>
+    <col min="23" max="23" width="103.111111111111" style="3" customWidth="1"/>
     <col min="24" max="16384" width="8.88888888888889" style="3"/>
   </cols>
   <sheetData>
@@ -1475,10 +1491,10 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1495,23 +1511,23 @@
       <c r="D2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>31</v>
@@ -1532,10 +1548,10 @@
         <v>36</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>38</v>
@@ -1544,13 +1560,13 @@
         <v>39</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" spans="1:23">
@@ -1563,27 +1579,29 @@
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>42</v>
@@ -1615,7 +1633,7 @@
       <c r="U3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="V3" s="3" t="s">
         <v>42</v>
       </c>
       <c r="W3" s="3" t="s">
@@ -1632,21 +1650,23 @@
       <c r="C4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>42</v>
@@ -1684,7 +1704,7 @@
       <c r="U4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="V4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="W4" s="3" t="s">
@@ -1692,7 +1712,7 @@
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="15" customHeight="1" spans="1:23">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1701,64 +1721,197 @@
       <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W5" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W5" s="2" t="s">
+    </row>
+    <row r="6" s="3" customFormat="1" spans="1:23">
+      <c r="A6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="1" spans="1:20">
+      <c r="A7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T7" s="2" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Popravke testova i dopuna podacima data
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9467"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="73">
   <si>
     <t>username</t>
   </si>
@@ -59,9 +59,6 @@
     <t>current_account_3_name</t>
   </si>
   <si>
-    <t>current_account_3_bban</t>
-  </si>
-  <si>
     <t>current_account_3_iban</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
   </si>
   <si>
     <t>205-9001007790944-88</t>
-  </si>
-  <si>
-    <t>205-9031004419532-81</t>
   </si>
   <si>
     <t>RS35 2059 0310 0441 9532 81</t>
@@ -1481,11 +1475,11 @@
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomRight" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
@@ -1498,7 +1492,8 @@
     <col min="6" max="7" width="33.8888888888889" style="3" customWidth="1"/>
     <col min="8" max="8" width="23.6666666666667" style="3" customWidth="1"/>
     <col min="9" max="9" width="28.7407407407407" style="3" customWidth="1"/>
-    <col min="10" max="11" width="24.2222222222222" style="3" customWidth="1"/>
+    <col min="10" max="10" width="24.2222222222222" style="3" customWidth="1"/>
+    <col min="11" max="11" width="27.8888888888889" style="3" customWidth="1"/>
     <col min="12" max="12" width="28.8611111111111" style="3" customWidth="1"/>
     <col min="13" max="13" width="24.2222222222222" style="3" customWidth="1"/>
     <col min="14" max="14" width="23.6666666666667" style="3" customWidth="1"/>
@@ -1553,592 +1548,592 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" spans="1:29">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="T2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="U2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="W2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="X2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="AB2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" spans="1:29">
       <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="I3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="L3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="Y3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" spans="1:29">
       <c r="A4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="M4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="15" customHeight="1" spans="1:29">
       <c r="A5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="I5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA5" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>64</v>
-      </c>
       <c r="AB5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" spans="1:29">
       <c r="A6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="J6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="N6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" s="2" t="s">
+      <c r="O6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB6" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="AC6" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC6" s="13" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:29">
       <c r="A7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="J7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AC7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Domestic Payments Modify Data zavrsetak
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="74">
   <si>
     <t>username</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Enil ČIĆVI</t>
+  </si>
+  <si>
+    <t>205-9001015647000-10</t>
   </si>
   <si>
     <t>RS35 2059 0310 0988 6201 58</t>
@@ -1475,11 +1478,11 @@
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M22" sqref="M22"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
@@ -1705,16 +1708,16 @@
         <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>31</v>
@@ -1723,10 +1726,10 @@
         <v>30</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>31</v>
@@ -1762,7 +1765,7 @@
         <v>44</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>31</v>
@@ -1782,7 +1785,7 @@
     </row>
     <row r="4" s="3" customFormat="1" spans="1:29">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>31</v>
@@ -1794,28 +1797,28 @@
         <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>31</v>
@@ -1871,7 +1874,7 @@
     </row>
     <row r="5" s="2" customFormat="1" ht="15" customHeight="1" spans="1:29">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>31</v>
@@ -1886,13 +1889,13 @@
         <v>31</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>31</v>
@@ -1949,7 +1952,7 @@
         <v>31</v>
       </c>
       <c r="AA5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AB5" s="2" t="s">
         <v>31</v>
@@ -1960,7 +1963,7 @@
     </row>
     <row r="6" s="3" customFormat="1" spans="1:29">
       <c r="A6" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>31</v>
@@ -1972,7 +1975,7 @@
         <v>33</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>31</v>
@@ -1984,7 +1987,7 @@
         <v>31</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>31</v>
@@ -1996,10 +1999,10 @@
         <v>31</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>31</v>
@@ -2041,15 +2044,15 @@
         <v>31</v>
       </c>
       <c r="AB6" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AC6" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:29">
       <c r="A7" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>31</v>
@@ -2061,7 +2064,7 @@
         <v>33</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>31</v>
@@ -2073,7 +2076,7 @@
         <v>31</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Popravke testova deposit lists i Show/Hide
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="13884" windowHeight="4356"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1478,11 +1478,11 @@
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>

</xml_diff>

<commit_message>
Nekoliko testova sitne ispravke, Payment in Future test..
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13884" windowHeight="4356"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="86">
   <si>
     <t>username</t>
   </si>
@@ -59,6 +59,9 @@
     <t>current_account_3_name</t>
   </si>
   <si>
+    <t>current_account_3_bban</t>
+  </si>
+  <si>
     <t>current_account_3_iban</t>
   </si>
   <si>
@@ -113,6 +116,27 @@
     <t>loan_account_1_number</t>
   </si>
   <si>
+    <t>user_name_for_payment_review</t>
+  </si>
+  <si>
+    <t>user_street_for_payment_review</t>
+  </si>
+  <si>
+    <t>user_city_for_payment_review</t>
+  </si>
+  <si>
+    <t>user_bban_for_payment_review</t>
+  </si>
+  <si>
+    <t>user_amount_for_payment_review</t>
+  </si>
+  <si>
+    <t>username_debtor_for_payment_review</t>
+  </si>
+  <si>
+    <t>user_address_for_payment_review</t>
+  </si>
+  <si>
     <t>Osir ANOEV</t>
   </si>
   <si>
@@ -170,6 +194,24 @@
     <t xml:space="preserve">Account type: Current account Account owner: OSIR ANOEV Account number: RS35 2059 0310 0441 7882 84 BIC: KOBBRSBG </t>
   </si>
   <si>
+    <t>PERA</t>
+  </si>
+  <si>
+    <t>ULICAA</t>
+  </si>
+  <si>
+    <t>BEOGRAD</t>
+  </si>
+  <si>
+    <t>205-9001001626239-86</t>
+  </si>
+  <si>
+    <t>ANOEV OSIR</t>
+  </si>
+  <si>
+    <t>ULICAA,BEOGRAD</t>
+  </si>
+  <si>
     <t>Enil ČIĆVI</t>
   </si>
   <si>
@@ -182,9 +224,6 @@
     <t>205-9001010537788-94</t>
   </si>
   <si>
-    <t>205-9031008901983-32</t>
-  </si>
-  <si>
     <t>RS35 2059 0310 0890 1983 32</t>
   </si>
   <si>
@@ -213,9 +252,6 @@
   </si>
   <si>
     <t>RS35 2059 0310 0263 7397 40</t>
-  </si>
-  <si>
-    <t>205-9001001626239-86</t>
   </si>
   <si>
     <t xml:space="preserve">Account type: Current account Account owner: DRRE ĆEVMI Account number: RS35 2059 0310 0263 7397 40 BIC: KOBBRSBG </t>
@@ -1475,14 +1511,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
@@ -1513,10 +1549,16 @@
     <col min="27" max="27" width="114.777777777778" style="3" customWidth="1"/>
     <col min="28" max="28" width="26.0092592592593" style="3" customWidth="1"/>
     <col min="29" max="29" width="23.5555555555556" style="3" customWidth="1"/>
-    <col min="30" max="16384" width="8.88888888888889" style="3"/>
+    <col min="30" max="30" width="31" style="3" customWidth="1"/>
+    <col min="31" max="32" width="32.8888888888889" style="3" customWidth="1"/>
+    <col min="33" max="33" width="29.1111111111111" style="3" customWidth="1"/>
+    <col min="34" max="34" width="33" style="3" customWidth="1"/>
+    <col min="35" max="35" width="37.1111111111111" style="3" customWidth="1"/>
+    <col min="36" max="36" width="31.2222222222222" style="3" customWidth="1"/>
+    <col min="37" max="16384" width="8.88888888888889" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:29">
+    <row r="1" s="1" customFormat="1" spans="1:36">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1551,592 +1593,634 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:29">
+    <row r="2" s="2" customFormat="1" spans="1:36">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="V2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="AA2" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>73</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" spans="1:29">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="L3" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="X3" s="2" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" spans="1:29">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="15" customHeight="1" spans="1:29">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AA5" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" spans="1:29">
       <c r="A6" s="8" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AB6" s="11" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="AC6" s="13" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:29">
       <c r="A7" s="8" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AC7" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ispravke pred pustanje testova 6.2.2026
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="89">
   <si>
     <t>username</t>
   </si>
@@ -107,9 +107,6 @@
     <t>default_account_bban</t>
   </si>
   <si>
-    <t>copied_account_details_for_personal_account</t>
-  </si>
-  <si>
     <t>loan_account_1_name</t>
   </si>
   <si>
@@ -137,6 +134,12 @@
     <t>user_address_for_payment_review</t>
   </si>
   <si>
+    <t>user_country_short</t>
+  </si>
+  <si>
+    <t>user_city_short</t>
+  </si>
+  <si>
     <t>Osir ANOEV</t>
   </si>
   <si>
@@ -161,6 +164,9 @@
     <t>RS35 2059 0310 0441 9532 81</t>
   </si>
   <si>
+    <t>RS35 2059 0310 0021 5320 98</t>
+  </si>
+  <si>
     <t>Visa prepaid</t>
   </si>
   <si>
@@ -191,9 +197,6 @@
     <t>9032022325800</t>
   </si>
   <si>
-    <t xml:space="preserve">Account type: Current account Account owner: OSIR ANOEV Account number: RS35 2059 0310 0441 7882 84 BIC: KOBBRSBG </t>
-  </si>
-  <si>
     <t>PERA</t>
   </si>
   <si>
@@ -212,6 +215,15 @@
     <t>ULICAA,BEOGRAD</t>
   </si>
   <si>
+    <t>SERBIA</t>
+  </si>
+  <si>
+    <t>KOAR TGR</t>
+  </si>
+  <si>
+    <t>Beograd</t>
+  </si>
+  <si>
     <t>Enil ČIĆVI</t>
   </si>
   <si>
@@ -252,9 +264,6 @@
   </si>
   <si>
     <t>RS35 2059 0310 0263 7397 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account type: Current account Account owner: DRRE ĆEVMI Account number: RS35 2059 0310 0263 7397 40 BIC: KOBBRSBG </t>
   </si>
   <si>
     <t>Jail ĆEVGIMILĆ</t>
@@ -1511,14 +1520,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AH2" sqref="AH2"/>
+      <selection pane="bottomRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
@@ -1546,19 +1555,21 @@
     <col min="24" max="24" width="32.1851851851852" style="3" customWidth="1"/>
     <col min="25" max="25" width="17.6666666666667" style="3" customWidth="1"/>
     <col min="26" max="26" width="23.8888888888889" style="3" customWidth="1"/>
-    <col min="27" max="27" width="114.777777777778" style="3" customWidth="1"/>
-    <col min="28" max="28" width="26.0092592592593" style="3" customWidth="1"/>
-    <col min="29" max="29" width="23.5555555555556" style="3" customWidth="1"/>
-    <col min="30" max="30" width="31" style="3" customWidth="1"/>
-    <col min="31" max="32" width="32.8888888888889" style="3" customWidth="1"/>
-    <col min="33" max="33" width="29.1111111111111" style="3" customWidth="1"/>
-    <col min="34" max="34" width="33" style="3" customWidth="1"/>
-    <col min="35" max="35" width="37.1111111111111" style="3" customWidth="1"/>
-    <col min="36" max="36" width="31.2222222222222" style="3" customWidth="1"/>
-    <col min="37" max="16384" width="8.88888888888889" style="3"/>
+    <col min="27" max="27" width="26.0092592592593" style="3" customWidth="1"/>
+    <col min="28" max="28" width="23.5555555555556" style="3" customWidth="1"/>
+    <col min="29" max="29" width="31" style="3" customWidth="1"/>
+    <col min="30" max="31" width="32.8888888888889" style="3" customWidth="1"/>
+    <col min="32" max="32" width="29.1111111111111" style="3" customWidth="1"/>
+    <col min="33" max="33" width="33" style="3" customWidth="1"/>
+    <col min="34" max="34" width="37.1111111111111" style="3" customWidth="1"/>
+    <col min="35" max="35" width="31.2222222222222" style="3" customWidth="1"/>
+    <col min="36" max="36" width="18.5555555555556" style="3" customWidth="1"/>
+    <col min="37" max="37" width="16.6666666666667" style="3" customWidth="1"/>
+    <col min="38" max="38" width="14.7777777777778" style="3" customWidth="1"/>
+    <col min="39" max="16384" width="8.88888888888889" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:36">
+    <row r="1" s="1" customFormat="1" spans="1:38">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1667,560 +1678,557 @@
       <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="AK1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:36">
+    <row r="2" s="2" customFormat="1" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>73</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" s="3" customFormat="1" spans="1:28">
+      <c r="A3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" s="3" customFormat="1" spans="1:28">
+      <c r="A4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z2" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="15" customHeight="1" spans="1:28">
+      <c r="A5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB2" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="1" spans="1:28">
+      <c r="A6" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="H6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB6" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="1" spans="1:28">
+      <c r="A7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AD2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG2" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>73</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" s="3" customFormat="1" spans="1:29">
-      <c r="A3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" s="3" customFormat="1" spans="1:29">
-      <c r="A4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" s="2" customFormat="1" ht="15" customHeight="1" spans="1:29">
-      <c r="A5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" s="3" customFormat="1" spans="1:29">
-      <c r="A6" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB6" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC6" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" s="3" customFormat="1" spans="1:29">
-      <c r="A7" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="H7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC7" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
popravke mnogih testova, uglavnom sitnije, multiper filter invalid...
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
   <si>
     <t>username</t>
   </si>
@@ -197,73 +197,70 @@
     <t>9032022325800</t>
   </si>
   <si>
-    <t>PERA</t>
+    <t>KOAR TGR</t>
   </si>
   <si>
     <t>ULICAA</t>
   </si>
   <si>
-    <t>BEOGRAD</t>
+    <t>Beograd</t>
+  </si>
+  <si>
+    <t>205-9001000243808-47</t>
+  </si>
+  <si>
+    <t>ANOEV OSIR</t>
+  </si>
+  <si>
+    <t>ULICAA,BEOGRAD</t>
+  </si>
+  <si>
+    <t>SERBIA</t>
+  </si>
+  <si>
+    <t>Enil ČIĆVI</t>
+  </si>
+  <si>
+    <t>205-9001015647000-10</t>
+  </si>
+  <si>
+    <t>RS35 2059 0310 0988 6201 58</t>
+  </si>
+  <si>
+    <t>205-9001010537788-94</t>
+  </si>
+  <si>
+    <t>RS35 2059 0310 0890 1983 32</t>
+  </si>
+  <si>
+    <t>205-9032030694661-90</t>
+  </si>
+  <si>
+    <t>Vklaragan OVIT</t>
+  </si>
+  <si>
+    <t>205-9001004906720-69</t>
+  </si>
+  <si>
+    <t>RS35 2059 0310 0233 1565 13</t>
+  </si>
+  <si>
+    <t>205-9031002331565-13</t>
+  </si>
+  <si>
+    <t>205-9031002328491-20</t>
+  </si>
+  <si>
+    <t>RS35 2059 0310 0232 8491 20</t>
+  </si>
+  <si>
+    <t>Drre ĆEVMI</t>
+  </si>
+  <si>
+    <t>RS35 2059 0310 0263 7397 40</t>
   </si>
   <si>
     <t>205-9001001626239-86</t>
-  </si>
-  <si>
-    <t>ANOEV OSIR</t>
-  </si>
-  <si>
-    <t>ULICAA,BEOGRAD</t>
-  </si>
-  <si>
-    <t>SERBIA</t>
-  </si>
-  <si>
-    <t>KOAR TGR</t>
-  </si>
-  <si>
-    <t>Beograd</t>
-  </si>
-  <si>
-    <t>Enil ČIĆVI</t>
-  </si>
-  <si>
-    <t>205-9001015647000-10</t>
-  </si>
-  <si>
-    <t>RS35 2059 0310 0988 6201 58</t>
-  </si>
-  <si>
-    <t>205-9001010537788-94</t>
-  </si>
-  <si>
-    <t>RS35 2059 0310 0890 1983 32</t>
-  </si>
-  <si>
-    <t>205-9032030694661-90</t>
-  </si>
-  <si>
-    <t>Vklaragan OVIT</t>
-  </si>
-  <si>
-    <t>205-9001004906720-69</t>
-  </si>
-  <si>
-    <t>RS35 2059 0310 0233 1565 13</t>
-  </si>
-  <si>
-    <t>205-9031002331565-13</t>
-  </si>
-  <si>
-    <t>205-9031002328491-20</t>
-  </si>
-  <si>
-    <t>RS35 2059 0310 0232 8491 20</t>
-  </si>
-  <si>
-    <t>Drre ĆEVMI</t>
-  </si>
-  <si>
-    <t>RS35 2059 0310 0263 7397 40</t>
   </si>
   <si>
     <t>Jail ĆEVGIMILĆ</t>
@@ -1523,11 +1520,11 @@
   <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X1" sqref="X1"/>
+      <selection pane="bottomRight" activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
@@ -1779,7 +1776,7 @@
       <c r="AE2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AF2" s="12" t="s">
+      <c r="AF2" s="2" t="s">
         <v>59</v>
       </c>
       <c r="AG2" s="2">
@@ -1795,15 +1792,15 @@
         <v>62</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" spans="1:28">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>40</v>
@@ -1815,16 +1812,16 @@
         <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>40</v>
@@ -1836,7 +1833,7 @@
         <v>40</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>40</v>
@@ -1872,7 +1869,7 @@
         <v>54</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>40</v>
@@ -1889,7 +1886,7 @@
     </row>
     <row r="4" s="3" customFormat="1" spans="1:28">
       <c r="A4" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>40</v>
@@ -1901,28 +1898,28 @@
         <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>39</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>40</v>
@@ -1975,7 +1972,7 @@
     </row>
     <row r="5" s="2" customFormat="1" ht="15" customHeight="1" spans="1:28">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>40</v>
@@ -1990,13 +1987,13 @@
         <v>40</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>40</v>
@@ -2061,7 +2058,7 @@
     </row>
     <row r="6" s="3" customFormat="1" spans="1:28">
       <c r="A6" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>40</v>
@@ -2073,7 +2070,7 @@
         <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
@@ -2085,69 +2082,69 @@
         <v>40</v>
       </c>
       <c r="I6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA6" s="11" t="s">
+      <c r="AB6" s="13" t="s">
         <v>84</v>
-      </c>
-      <c r="AB6" s="13" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:28">
       <c r="A7" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>40</v>
@@ -2159,7 +2156,7 @@
         <v>42</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>40</v>
@@ -2171,7 +2168,7 @@
         <v>40</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>40</v>

</xml_diff>